<commit_message>
criacao-formulario - Desenvolvendo geração do excel
</commit_message>
<xml_diff>
--- a/Excel/Modelo.xlsx
+++ b/Excel/Modelo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\Levantoso\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3CEABA-88B2-4E60-95A0-A82B39CDB634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341797EA-0EBE-4FA7-A9AF-4DB8FC30A843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1685E115-3842-4B19-9AA7-2E5C85CC0CEE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1685E115-3842-4B19-9AA7-2E5C85CC0CEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Levantamento de horas" sheetId="1" r:id="rId1"/>
@@ -201,7 +201,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -342,80 +342,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -424,19 +394,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -444,13 +405,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -785,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A05740DD-6BFA-4189-9EF4-A33BF1EFB91B}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,100 +820,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="24" x14ac:dyDescent="0.4">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
-      <c r="I1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="3"/>
+      <c r="A1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="25"/>
+      <c r="I1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="25"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="27"/>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="37"/>
-      <c r="K2" s="6" t="s">
+      <c r="J2" s="27"/>
+      <c r="K2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="9" t="s">
+      <c r="A3" s="30"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="6" t="s">
+      <c r="F3" s="34"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="15" t="s">
+      <c r="A4" s="28"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="I4" s="16" t="s">
+      <c r="F4" s="35"/>
+      <c r="I4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="36"/>
-      <c r="K4" s="15" t="s">
+      <c r="J4" s="17"/>
+      <c r="K4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="L4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="15" t="s">
+      <c r="M4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -913,313 +924,349 @@
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
       <c r="F5" s="20"/>
-      <c r="I5" s="21" t="s">
+      <c r="I5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="22" t="s">
+      <c r="J5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="15">
+      <c r="K5" s="5">
         <v>1</v>
       </c>
-      <c r="L5" s="15">
+      <c r="L5" s="5">
         <v>3</v>
       </c>
-      <c r="M5" s="15">
+      <c r="M5" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="22" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5">
+        <f>(C6*$K$5)+(D6*$L$5)+(E6*$M$5)</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="15">
+      <c r="K6" s="5">
         <v>1</v>
       </c>
-      <c r="L6" s="15">
+      <c r="L6" s="5">
         <v>3</v>
       </c>
-      <c r="M6" s="15">
+      <c r="M6" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="22" t="s">
+      <c r="A7" s="33"/>
+      <c r="B7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="I7" s="21" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5">
+        <f>(C7*$K$6)+(D7*$L$6)+(E7*$M$6)</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="22" t="s">
+      <c r="J7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K7" s="5">
         <v>3</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7" s="5">
         <v>8</v>
       </c>
-      <c r="M7" s="15">
+      <c r="M7" s="5">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="22" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5">
+        <f>(C8*$K$6)+(D8*$L$6)+(E8*$M$6)</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="15">
+      <c r="K8" s="5">
         <v>3</v>
       </c>
-      <c r="L8" s="15">
+      <c r="L8" s="5">
         <v>8</v>
       </c>
-      <c r="M8" s="15">
+      <c r="M8" s="5">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
-      <c r="B9" s="22" t="s">
+      <c r="A9" s="33"/>
+      <c r="B9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="I9" s="26" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5">
+        <f>(C9*$K$8)+(D9*$L$8)+(E9*$M$8)</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="27" t="s">
+      <c r="J9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="28">
+      <c r="K9" s="12">
         <v>1</v>
       </c>
-      <c r="L9" s="28">
+      <c r="L9" s="12">
         <v>4</v>
       </c>
-      <c r="M9" s="28">
+      <c r="M9" s="12">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="22" t="s">
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5">
+        <f>(C10*$K$9)+(D10*$L$9)+(E10*$M$9)</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="15">
+      <c r="K10" s="5">
         <v>2</v>
       </c>
-      <c r="L10" s="15">
+      <c r="L10" s="5">
         <v>5</v>
       </c>
-      <c r="M10" s="15">
+      <c r="M10" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
-      <c r="B11" s="22" t="s">
+      <c r="A11" s="36"/>
+      <c r="B11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="22" t="s">
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5">
+        <f>(C11*$K$10)+(D11*$L$10)+(E11*$M$10)</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="7"/>
+      <c r="J11" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="15">
+      <c r="K11" s="5">
         <v>1</v>
       </c>
-      <c r="L11" s="15">
+      <c r="L11" s="5">
         <v>3</v>
       </c>
-      <c r="M11" s="15">
+      <c r="M11" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
-      <c r="B12" s="22" t="s">
+      <c r="A12" s="36"/>
+      <c r="B12" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="22" t="s">
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5">
+        <f>(C12*$K$11)+(D12*$L$11)+(E12*$M$11)</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K12" s="15">
+      <c r="K12" s="5">
         <v>1</v>
       </c>
-      <c r="L12" s="15">
+      <c r="L12" s="5">
         <v>3</v>
       </c>
-      <c r="M12" s="15">
+      <c r="M12" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
-      <c r="B13" s="22" t="s">
+      <c r="A13" s="36"/>
+      <c r="B13" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="22" t="s">
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5">
+        <f>(C13*$K$12)+(D13*$L$12)+(E13*$M$12)</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K13" s="15">
+      <c r="K13" s="5">
         <v>1</v>
       </c>
-      <c r="L13" s="15">
+      <c r="L13" s="5">
         <v>3</v>
       </c>
-      <c r="M13" s="15">
+      <c r="M13" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
-      <c r="B14" s="22" t="s">
+      <c r="A14" s="36"/>
+      <c r="B14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="30" t="s">
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5">
+        <f>(C14*$K$13)+(D14*$L$13)+(E14*$M$13)</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="7"/>
+      <c r="J14" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="K14" s="15">
+      <c r="K14" s="5">
         <v>1</v>
       </c>
-      <c r="L14" s="15">
+      <c r="L14" s="5">
         <v>3</v>
       </c>
-      <c r="M14" s="15">
+      <c r="M14" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="22" t="s">
+      <c r="A15" s="33"/>
+      <c r="B15" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="I15" s="21" t="s">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5">
+        <f>(C15*$K$14)+(D15*$L$14)+(E15*$M$14)</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="22" t="s">
+      <c r="J15" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K15" s="15">
+      <c r="K15" s="5">
         <v>1</v>
       </c>
-      <c r="L15" s="15">
+      <c r="L15" s="5">
         <v>3</v>
       </c>
-      <c r="M15" s="15">
+      <c r="M15" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="I16" s="21" t="s">
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5">
+        <f>(C16*$K$15)+(D16*$L$15)+(E16*$M$15)</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="J16" s="22" t="s">
+      <c r="J16" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K16" s="15">
+      <c r="K16" s="5">
         <v>3</v>
       </c>
-      <c r="L16" s="15">
+      <c r="L16" s="5">
         <v>8</v>
       </c>
-      <c r="M16" s="15">
+      <c r="M16" s="5">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="I17" s="25"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5">
+        <f>(C17*$K$16)+(D17*$L$16)+(E17*$M$16)</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="34">
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="15">
         <f>SUM(F6:F17)</f>
         <v>0</v>
       </c>
@@ -1231,28 +1278,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O23" s="39"/>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="10">
     <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A15"/>
     <mergeCell ref="A18:E18"/>
     <mergeCell ref="I1:M1"/>
     <mergeCell ref="I2:J3"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:B4"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A10:A15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>